<commit_message>
supp tables and typos
</commit_message>
<xml_diff>
--- a/results/supplement/tables/Table_S1.xlsx
+++ b/results/supplement/tables/Table_S1.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Statistical summary (antibiotics)" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Statistical summary (infection)" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t xml:space="preserve">Antibiotic</t>
   </si>
@@ -89,6 +91,231 @@
   </si>
   <si>
     <t xml:space="preserve">10 mg/kg body weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effect of antibiotics on community structure:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inverse Simpson Diversity (median)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inverse Simpson Diversity (Q25-Q75)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Inverse Simpson Diversity vs Untreated (</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">p</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-value)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Bray-Curtis from Untreated (median)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bray-Curtis from Untreated (Q25-Q75)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bray-Curtis vs Untreated (</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">p</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-value)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Untreated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.645 – 13.646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.066 – 1.105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.961 – 0.985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.79 – 4.041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.747 – 0.927</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.283 – 1.429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.983 – 0.991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effect of antibiotics on metabolome:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.831 – 0.865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.764 – 0.833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.84 – 0.869</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effect of infection on community structure:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Inverse Simpson Diversity vs Mock (</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">p</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-value)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Bray-Curtis from Mock (median)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bray-Curtis from Mock (Q25-Q75)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bray-Curtis vs Mock (</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <i val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">p</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="FreeSans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-value)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1.175 - 1.405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.061 - 0.146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.378 - 4.538</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.452 - 0.978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.171 - 1.269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.094 - 0.156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effect of infection on metabolome:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.241- 0.375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.387 - 0.489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.236 - 0.327</t>
   </si>
 </sst>
 </file>
@@ -98,11 +325,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,6 +375,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="FreeSans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -162,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -185,6 +428,13 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -211,7 +461,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -230,6 +480,54 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -311,19 +609,19 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.1275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="77.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="68.8826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="76.6734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="68.0357142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,4 +713,429 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="40.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="34.0102040816326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="44.4285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="34.3622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="31.234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="5" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>12.65</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="13" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>0.979</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="9" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="14" t="n">
+        <v>3.195</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="13" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="9" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>1.372</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="13" t="n">
+        <v>0.0006</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>0.987</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>0.848</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>0.808</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>0.854</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="32.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="34.0102040816326"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="40.6122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="34.3622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="31.234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="5" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="15" t="n">
+        <v>1.326</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="13" t="n">
+        <v>0.0108</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="16" t="n">
+        <v>0.065</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="15" t="n">
+        <v>2.976</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="16" t="n">
+        <v>0.9616</v>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="13" t="n">
+        <v>0.038</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>1.186</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="16" t="n">
+        <v>0.0934</v>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="13" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>0.294</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="13" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="16" t="n">
+        <v>0.092</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="16" t="n">
+        <v>0.159</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>